<commit_message>
update reports and plant
</commit_message>
<xml_diff>
--- a/Documents/Template QLDA.xlsx
+++ b/Documents/Template QLDA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicotine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicotine/N06-PTTKPM-NHOM3/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30186868-4B23-BE42-870C-B62AE1933B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345804D4-2B20-3540-B63A-1203B0677AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -1164,22 +1164,19 @@
     <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1191,14 +1188,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1800,8 +1800,8 @@
   </sheetPr>
   <dimension ref="A1:BL45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1827,28 +1827,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="128" t="s">
+      <c r="I1" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="127">
+      <c r="Q1" s="126">
         <v>45644</v>
       </c>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="126"/>
-      <c r="Y1" s="126"/>
-      <c r="Z1" s="126"/>
+      <c r="R1" s="125"/>
+      <c r="S1" s="125"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="125"/>
+      <c r="X1" s="125"/>
+      <c r="Y1" s="125"/>
+      <c r="Z1" s="125"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="96" t="s">
@@ -1860,28 +1860,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="128" t="s">
+      <c r="I2" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="125">
+      <c r="Q2" s="124">
         <v>1</v>
       </c>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="126"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
     </row>
     <row r="3" spans="1:64" ht="26" x14ac:dyDescent="0.4">
       <c r="B3" s="96" t="s">
@@ -1977,102 +1977,102 @@
       <c r="A7" s="14"/>
       <c r="B7" s="29"/>
       <c r="E7" s="30"/>
-      <c r="I7" s="132">
+      <c r="I7" s="121">
         <f>I8</f>
         <v>45642</v>
       </c>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
-      <c r="N7" s="130"/>
-      <c r="O7" s="130"/>
-      <c r="P7" s="130">
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="119">
         <f>P8</f>
         <v>45649</v>
       </c>
-      <c r="Q7" s="130"/>
-      <c r="R7" s="130"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="130"/>
-      <c r="U7" s="130"/>
-      <c r="V7" s="130"/>
-      <c r="W7" s="130">
+      <c r="Q7" s="119"/>
+      <c r="R7" s="119"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="119"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="119">
         <f>W8</f>
         <v>45656</v>
       </c>
-      <c r="X7" s="130"/>
-      <c r="Y7" s="130"/>
-      <c r="Z7" s="130"/>
-      <c r="AA7" s="130"/>
-      <c r="AB7" s="130"/>
-      <c r="AC7" s="130"/>
-      <c r="AD7" s="130">
+      <c r="X7" s="119"/>
+      <c r="Y7" s="119"/>
+      <c r="Z7" s="119"/>
+      <c r="AA7" s="119"/>
+      <c r="AB7" s="119"/>
+      <c r="AC7" s="119"/>
+      <c r="AD7" s="119">
         <f>AD8</f>
         <v>45663</v>
       </c>
-      <c r="AE7" s="130"/>
-      <c r="AF7" s="130"/>
-      <c r="AG7" s="130"/>
-      <c r="AH7" s="130"/>
-      <c r="AI7" s="130"/>
-      <c r="AJ7" s="130"/>
-      <c r="AK7" s="130">
+      <c r="AE7" s="119"/>
+      <c r="AF7" s="119"/>
+      <c r="AG7" s="119"/>
+      <c r="AH7" s="119"/>
+      <c r="AI7" s="119"/>
+      <c r="AJ7" s="119"/>
+      <c r="AK7" s="119">
         <f>AK8</f>
         <v>45670</v>
       </c>
-      <c r="AL7" s="130"/>
-      <c r="AM7" s="130"/>
-      <c r="AN7" s="130"/>
-      <c r="AO7" s="130"/>
-      <c r="AP7" s="130"/>
-      <c r="AQ7" s="130"/>
-      <c r="AR7" s="130">
+      <c r="AL7" s="119"/>
+      <c r="AM7" s="119"/>
+      <c r="AN7" s="119"/>
+      <c r="AO7" s="119"/>
+      <c r="AP7" s="119"/>
+      <c r="AQ7" s="119"/>
+      <c r="AR7" s="119">
         <f>AR8</f>
         <v>45677</v>
       </c>
-      <c r="AS7" s="130"/>
-      <c r="AT7" s="130"/>
-      <c r="AU7" s="130"/>
-      <c r="AV7" s="130"/>
-      <c r="AW7" s="130"/>
-      <c r="AX7" s="130"/>
-      <c r="AY7" s="130">
+      <c r="AS7" s="119"/>
+      <c r="AT7" s="119"/>
+      <c r="AU7" s="119"/>
+      <c r="AV7" s="119"/>
+      <c r="AW7" s="119"/>
+      <c r="AX7" s="119"/>
+      <c r="AY7" s="119">
         <f>AY8</f>
         <v>45684</v>
       </c>
-      <c r="AZ7" s="130"/>
-      <c r="BA7" s="130"/>
-      <c r="BB7" s="130"/>
-      <c r="BC7" s="130"/>
-      <c r="BD7" s="130"/>
-      <c r="BE7" s="130"/>
-      <c r="BF7" s="130">
+      <c r="AZ7" s="119"/>
+      <c r="BA7" s="119"/>
+      <c r="BB7" s="119"/>
+      <c r="BC7" s="119"/>
+      <c r="BD7" s="119"/>
+      <c r="BE7" s="119"/>
+      <c r="BF7" s="119">
         <f>BF8</f>
         <v>45691</v>
       </c>
-      <c r="BG7" s="130"/>
-      <c r="BH7" s="130"/>
-      <c r="BI7" s="130"/>
-      <c r="BJ7" s="130"/>
-      <c r="BK7" s="130"/>
-      <c r="BL7" s="131"/>
+      <c r="BG7" s="119"/>
+      <c r="BH7" s="119"/>
+      <c r="BI7" s="119"/>
+      <c r="BJ7" s="119"/>
+      <c r="BK7" s="119"/>
+      <c r="BL7" s="120"/>
     </row>
     <row r="8" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="119"/>
-      <c r="B8" s="120" t="s">
+      <c r="A8" s="129"/>
+      <c r="B8" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="124" t="s">
+      <c r="D8" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="124" t="s">
+      <c r="E8" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="124" t="s">
+      <c r="F8" s="122" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="31">
@@ -2301,8 +2301,8 @@
       </c>
     </row>
     <row r="9" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="119"/>
-      <c r="B9" s="121"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="123"/>
       <c r="D9" s="123"/>
       <c r="E9" s="123"/>
@@ -3083,9 +3083,7 @@
       <c r="B18" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="63" t="s">
-        <v>21</v>
-      </c>
+      <c r="C18" s="63"/>
       <c r="D18" s="64">
         <v>0.5</v>
       </c>
@@ -3164,9 +3162,7 @@
       <c r="B19" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="63" t="s">
-        <v>22</v>
-      </c>
+      <c r="C19" s="63"/>
       <c r="D19" s="64">
         <v>0.5</v>
       </c>
@@ -3245,9 +3241,7 @@
       <c r="B20" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="63" t="s">
-        <v>23</v>
-      </c>
+      <c r="C20" s="63"/>
       <c r="D20" s="64"/>
       <c r="E20" s="65">
         <f>F19</f>
@@ -3324,9 +3318,7 @@
       <c r="B21" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="63" t="s">
-        <v>24</v>
-      </c>
+      <c r="C21" s="63"/>
       <c r="D21" s="64"/>
       <c r="E21" s="65">
         <f>E20</f>
@@ -3403,9 +3395,7 @@
       <c r="B22" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="63" t="s">
-        <v>25</v>
-      </c>
+      <c r="C22" s="63"/>
       <c r="D22" s="64"/>
       <c r="E22" s="65">
         <f>E21</f>
@@ -3498,7 +3488,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="116" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D24" s="117">
         <v>0.5</v>
@@ -3579,7 +3569,7 @@
         <v>52</v>
       </c>
       <c r="C25" s="116" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="D25" s="117">
         <v>0.5</v>
@@ -3660,7 +3650,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="116" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D26" s="117"/>
       <c r="E26" s="118">
@@ -3739,7 +3729,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="116" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D27" s="117"/>
       <c r="E27" s="118">
@@ -3818,7 +3808,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="116" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D28" s="117"/>
       <c r="E28" s="118">
@@ -4965,6 +4955,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF7:BL7"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="P7:V7"/>
@@ -4973,16 +4973,6 @@
     <mergeCell ref="AK7:AQ7"/>
     <mergeCell ref="AR7:AX7"/>
     <mergeCell ref="AY7:BE7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:D42">
     <cfRule type="dataBar" priority="23">
@@ -5230,15 +5220,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5550,6 +5531,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -5570,14 +5560,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5598,6 +5580,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
update planning + srs tuan3 + fix t1 va t2
</commit_message>
<xml_diff>
--- a/Documents/Template QLDA.xlsx
+++ b/Documents/Template QLDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicotine/N06-PTTKPM-NHOM3/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345804D4-2B20-3540-B63A-1203B0677AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE2CAD9-492C-B245-AB0D-CD5FB575C233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1164,19 +1164,22 @@
     <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1188,17 +1191,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1801,7 +1801,7 @@
   <dimension ref="A1:BL45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1827,28 +1827,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="127" t="s">
+      <c r="I1" s="128" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="126">
+      <c r="Q1" s="127">
         <v>45644</v>
       </c>
-      <c r="R1" s="125"/>
-      <c r="S1" s="125"/>
-      <c r="T1" s="125"/>
-      <c r="U1" s="125"/>
-      <c r="V1" s="125"/>
-      <c r="W1" s="125"/>
-      <c r="X1" s="125"/>
-      <c r="Y1" s="125"/>
-      <c r="Z1" s="125"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="126"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="96" t="s">
@@ -1860,28 +1860,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="127" t="s">
+      <c r="I2" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="124">
+      <c r="Q2" s="125">
         <v>1</v>
       </c>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
+      <c r="R2" s="126"/>
+      <c r="S2" s="126"/>
+      <c r="T2" s="126"/>
+      <c r="U2" s="126"/>
+      <c r="V2" s="126"/>
+      <c r="W2" s="126"/>
+      <c r="X2" s="126"/>
+      <c r="Y2" s="126"/>
+      <c r="Z2" s="126"/>
     </row>
     <row r="3" spans="1:64" ht="26" x14ac:dyDescent="0.4">
       <c r="B3" s="96" t="s">
@@ -1977,102 +1977,102 @@
       <c r="A7" s="14"/>
       <c r="B7" s="29"/>
       <c r="E7" s="30"/>
-      <c r="I7" s="121">
+      <c r="I7" s="132">
         <f>I8</f>
         <v>45642</v>
       </c>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
-      <c r="O7" s="119"/>
-      <c r="P7" s="119">
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130">
         <f>P8</f>
         <v>45649</v>
       </c>
-      <c r="Q7" s="119"/>
-      <c r="R7" s="119"/>
-      <c r="S7" s="119"/>
-      <c r="T7" s="119"/>
-      <c r="U7" s="119"/>
-      <c r="V7" s="119"/>
-      <c r="W7" s="119">
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="130"/>
+      <c r="T7" s="130"/>
+      <c r="U7" s="130"/>
+      <c r="V7" s="130"/>
+      <c r="W7" s="130">
         <f>W8</f>
         <v>45656</v>
       </c>
-      <c r="X7" s="119"/>
-      <c r="Y7" s="119"/>
-      <c r="Z7" s="119"/>
-      <c r="AA7" s="119"/>
-      <c r="AB7" s="119"/>
-      <c r="AC7" s="119"/>
-      <c r="AD7" s="119">
+      <c r="X7" s="130"/>
+      <c r="Y7" s="130"/>
+      <c r="Z7" s="130"/>
+      <c r="AA7" s="130"/>
+      <c r="AB7" s="130"/>
+      <c r="AC7" s="130"/>
+      <c r="AD7" s="130">
         <f>AD8</f>
         <v>45663</v>
       </c>
-      <c r="AE7" s="119"/>
-      <c r="AF7" s="119"/>
-      <c r="AG7" s="119"/>
-      <c r="AH7" s="119"/>
-      <c r="AI7" s="119"/>
-      <c r="AJ7" s="119"/>
-      <c r="AK7" s="119">
+      <c r="AE7" s="130"/>
+      <c r="AF7" s="130"/>
+      <c r="AG7" s="130"/>
+      <c r="AH7" s="130"/>
+      <c r="AI7" s="130"/>
+      <c r="AJ7" s="130"/>
+      <c r="AK7" s="130">
         <f>AK8</f>
         <v>45670</v>
       </c>
-      <c r="AL7" s="119"/>
-      <c r="AM7" s="119"/>
-      <c r="AN7" s="119"/>
-      <c r="AO7" s="119"/>
-      <c r="AP7" s="119"/>
-      <c r="AQ7" s="119"/>
-      <c r="AR7" s="119">
+      <c r="AL7" s="130"/>
+      <c r="AM7" s="130"/>
+      <c r="AN7" s="130"/>
+      <c r="AO7" s="130"/>
+      <c r="AP7" s="130"/>
+      <c r="AQ7" s="130"/>
+      <c r="AR7" s="130">
         <f>AR8</f>
         <v>45677</v>
       </c>
-      <c r="AS7" s="119"/>
-      <c r="AT7" s="119"/>
-      <c r="AU7" s="119"/>
-      <c r="AV7" s="119"/>
-      <c r="AW7" s="119"/>
-      <c r="AX7" s="119"/>
-      <c r="AY7" s="119">
+      <c r="AS7" s="130"/>
+      <c r="AT7" s="130"/>
+      <c r="AU7" s="130"/>
+      <c r="AV7" s="130"/>
+      <c r="AW7" s="130"/>
+      <c r="AX7" s="130"/>
+      <c r="AY7" s="130">
         <f>AY8</f>
         <v>45684</v>
       </c>
-      <c r="AZ7" s="119"/>
-      <c r="BA7" s="119"/>
-      <c r="BB7" s="119"/>
-      <c r="BC7" s="119"/>
-      <c r="BD7" s="119"/>
-      <c r="BE7" s="119"/>
-      <c r="BF7" s="119">
+      <c r="AZ7" s="130"/>
+      <c r="BA7" s="130"/>
+      <c r="BB7" s="130"/>
+      <c r="BC7" s="130"/>
+      <c r="BD7" s="130"/>
+      <c r="BE7" s="130"/>
+      <c r="BF7" s="130">
         <f>BF8</f>
         <v>45691</v>
       </c>
-      <c r="BG7" s="119"/>
-      <c r="BH7" s="119"/>
-      <c r="BI7" s="119"/>
-      <c r="BJ7" s="119"/>
-      <c r="BK7" s="119"/>
-      <c r="BL7" s="120"/>
+      <c r="BG7" s="130"/>
+      <c r="BH7" s="130"/>
+      <c r="BI7" s="130"/>
+      <c r="BJ7" s="130"/>
+      <c r="BK7" s="130"/>
+      <c r="BL7" s="131"/>
     </row>
     <row r="8" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="129"/>
-      <c r="B8" s="130" t="s">
+      <c r="A8" s="119"/>
+      <c r="B8" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="132" t="s">
+      <c r="C8" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="122" t="s">
+      <c r="D8" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="122" t="s">
+      <c r="E8" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="122" t="s">
+      <c r="F8" s="124" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="31">
@@ -2301,8 +2301,8 @@
       </c>
     </row>
     <row r="9" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="129"/>
-      <c r="B9" s="131"/>
+      <c r="A9" s="119"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="123"/>
       <c r="D9" s="123"/>
       <c r="E9" s="123"/>
@@ -2760,7 +2760,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="54">
         <v>0.6</v>
@@ -2841,7 +2841,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="53" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="54">
         <v>0.5</v>
@@ -3958,7 +3958,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="73" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="D30" s="74">
         <v>0.5</v>
@@ -4039,7 +4039,7 @@
         <v>40</v>
       </c>
       <c r="C31" s="73" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D31" s="74">
         <v>0.6</v>
@@ -4955,16 +4955,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF7:BL7"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="P7:V7"/>
@@ -4973,6 +4963,16 @@
     <mergeCell ref="AK7:AQ7"/>
     <mergeCell ref="AR7:AX7"/>
     <mergeCell ref="AY7:BE7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:D42">
     <cfRule type="dataBar" priority="23">
@@ -5220,6 +5220,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5531,15 +5540,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -5560,6 +5560,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5580,14 +5588,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>